<commit_message>
Now fixing RUS EST Heat data for 1990-1992/3
</commit_message>
<xml_diff>
--- a/data-raw/FixedRUSESTHeat19901993.xlsx
+++ b/data-raw/FixedRUSESTHeat19901993.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1614C143-FF55-E446-9D87-DEC52FB954E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC8AF25-09CA-FF44-9071-3EB922687ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="45640" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="45640" windowHeight="28180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -1256,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEDCB0B-213C-AD4A-9376-DC95417C0D54}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
@@ -6702,7 +6702,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8462,8 +8462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3863BE12-968E-D34A-ABE0-3AC81C7830A5}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>